<commit_message>
Indicadores e Cargas Bloco Imunizacao
</commit_message>
<xml_diff>
--- a/Entregaveis/1.RepositorioSemantico/Imunizacao/ConceptMap/brimunobiogico-sct_eng.xlsx
+++ b/Entregaveis/1.RepositorioSemantico/Imunizacao/ConceptMap/brimunobiogico-sct_eng.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beatrizdefarialeao/Documents/GitHub/ips-brasil-documentos/Entregaveis/1.RepositorioSemantico/Imunizacao/ConceptMap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B710BA74-76FB-B34D-BF80-8D458FEF1989}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE443C28-0A4B-1D47-95F8-D86D5E1FE475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="760" windowWidth="29360" windowHeight="17860" xr2:uid="{F59DAF0E-B1FE-DC47-A5F4-187CB422FD94}"/>
+    <workbookView xWindow="880" yWindow="760" windowWidth="29360" windowHeight="17860" activeTab="1" xr2:uid="{F59DAF0E-B1FE-DC47-A5F4-187CB422FD94}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping" sheetId="1" r:id="rId1"/>
@@ -1153,9 +1153,6 @@
     <t>(pentavalent) antivenom for Bothrops and Crotalus snake</t>
   </si>
   <si>
-    <t>pentavalent antivenom for Bothrops snakes and antilachetic snakes</t>
-  </si>
-  <si>
     <t>"trivalent antivenom for Loxosceles spiders</t>
   </si>
   <si>
@@ -1249,6 +1246,9 @@
   </si>
   <si>
     <t>Total Geral</t>
+  </si>
+  <si>
+    <t>pentavalent antivenom for  antilachetic snakes</t>
   </si>
 </sst>
 </file>
@@ -1542,7 +1542,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1598,24 +1598,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1629,9 +1611,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1652,9 +1631,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1681,14 +1657,14 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="12" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1709,9 +1685,6 @@
     <xf numFmtId="0" fontId="12" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1730,7 +1703,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1739,7 +1712,7 @@
     <xf numFmtId="0" fontId="13" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="14" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1775,10 +1748,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1796,8 +1766,29 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2117,7 +2108,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:J1046727"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="131" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="131" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -2147,7 +2138,7 @@
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
-      <c r="G1" s="62"/>
+      <c r="G1" s="53"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
@@ -2167,7 +2158,7 @@
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
-      <c r="G2" s="62"/>
+      <c r="G2" s="53"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
@@ -2191,7 +2182,7 @@
       <c r="F3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="35" t="s">
+      <c r="G3" s="28" t="s">
         <v>14</v>
       </c>
       <c r="H3" s="5" t="s">
@@ -2215,22 +2206,22 @@
         <v>18</v>
       </c>
       <c r="D4" s="7"/>
-      <c r="E4" s="86" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="88" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" s="30" t="s">
+      <c r="E4" s="76" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="78" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="H4" s="30" t="s">
+      <c r="H4" s="9" t="s">
         <v>197</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>396</v>
-      </c>
-      <c r="J4" s="87" t="s">
+        <v>395</v>
+      </c>
+      <c r="J4" s="77" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2241,7 +2232,7 @@
       <c r="B5" s="8">
         <v>5</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="20" t="s">
         <v>24</v>
       </c>
       <c r="D5" s="7" t="s">
@@ -2298,35 +2289,35 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="29" customFormat="1" ht="51" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="27">
+    <row r="7" spans="1:10" s="23" customFormat="1" ht="51" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="21">
         <v>10</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" s="28" t="s">
+      <c r="D7" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="H7" s="28" t="s">
+      <c r="H7" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="I7" s="27" t="s">
+      <c r="I7" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="J7" s="27" t="s">
+      <c r="J7" s="21" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2395,28 +2386,28 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="51" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="53" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="52">
+      <c r="A10" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="44">
         <v>15</v>
       </c>
-      <c r="C10" s="52" t="s">
+      <c r="C10" s="44" t="s">
         <v>218</v>
       </c>
-      <c r="D10" s="54"/>
-      <c r="E10" s="54"/>
-      <c r="F10" s="54"/>
-      <c r="G10" s="31" t="s">
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="24" t="s">
         <v>194</v>
       </c>
-      <c r="H10" s="31" t="s">
+      <c r="H10" s="24" t="s">
         <v>178</v>
       </c>
-      <c r="I10" s="89" t="s">
-        <v>395</v>
-      </c>
-      <c r="J10" s="67" t="s">
+      <c r="I10" s="79" t="s">
+        <v>394</v>
+      </c>
+      <c r="J10" s="58" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2456,29 +2447,29 @@
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="52">
+      <c r="B12" s="44">
         <v>18</v>
       </c>
-      <c r="C12" s="52" t="s">
+      <c r="C12" s="44" t="s">
         <v>217</v>
       </c>
-      <c r="D12" s="54"/>
-      <c r="E12" s="54" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="54" t="s">
-        <v>7</v>
-      </c>
-      <c r="G12" s="63">
+      <c r="D12" s="46"/>
+      <c r="E12" s="46" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="54">
         <v>871726005</v>
       </c>
-      <c r="H12" s="31" t="s">
+      <c r="H12" s="24" t="s">
         <v>181</v>
       </c>
       <c r="I12" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="J12" s="84" t="s">
+      <c r="J12" s="12" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2518,25 +2509,25 @@
       <c r="A14" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="66">
+      <c r="B14" s="57">
         <v>22</v>
       </c>
-      <c r="C14" s="66" t="s">
+      <c r="C14" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="66" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="F14" s="52" t="s">
-        <v>7</v>
-      </c>
-      <c r="G14" s="31" t="s">
+      <c r="D14" s="57" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" s="24" t="s">
         <v>198</v>
       </c>
-      <c r="H14" s="31" t="s">
+      <c r="H14" s="24" t="s">
         <v>199</v>
       </c>
       <c r="I14" s="7" t="s">
@@ -2550,25 +2541,25 @@
       <c r="A15" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="52">
+      <c r="B15" s="44">
         <v>23</v>
       </c>
-      <c r="C15" s="56" t="s">
+      <c r="C15" s="48" t="s">
         <v>253</v>
       </c>
-      <c r="D15" s="54"/>
-      <c r="E15" s="54"/>
-      <c r="F15" s="54"/>
-      <c r="G15" s="57" t="s">
+      <c r="D15" s="46"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="49" t="s">
         <v>221</v>
       </c>
-      <c r="H15" s="58" t="s">
+      <c r="H15" s="50" t="s">
         <v>187</v>
       </c>
-      <c r="I15" s="90" t="s">
-        <v>396</v>
-      </c>
-      <c r="J15" s="91" t="s">
+      <c r="I15" s="80" t="s">
+        <v>395</v>
+      </c>
+      <c r="J15" s="81" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2604,35 +2595,35 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="34" customFormat="1" ht="102" x14ac:dyDescent="0.2">
-      <c r="A17" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="26">
+    <row r="17" spans="1:10" s="27" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A17" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="20">
         <v>25</v>
       </c>
-      <c r="C17" s="26" t="s">
+      <c r="C17" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="D17" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="F17" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="G17" s="32" t="s">
+      <c r="D17" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="H17" s="33" t="s">
+      <c r="H17" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="I17" s="26" t="s">
+      <c r="I17" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="J17" s="26" t="s">
+      <c r="J17" s="20" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2640,25 +2631,25 @@
       <c r="A18" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="52">
+      <c r="B18" s="44">
         <v>26</v>
       </c>
-      <c r="C18" s="52" t="s">
+      <c r="C18" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="D18" s="52" t="s">
-        <v>19</v>
-      </c>
-      <c r="E18" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="F18" s="52" t="s">
-        <v>7</v>
-      </c>
-      <c r="G18" s="31" t="s">
+      <c r="D18" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18" s="24" t="s">
         <v>200</v>
       </c>
-      <c r="H18" s="31" t="s">
+      <c r="H18" s="24" t="s">
         <v>201</v>
       </c>
       <c r="I18" s="7" t="s">
@@ -2739,22 +2730,22 @@
       <c r="B21" s="8">
         <v>30</v>
       </c>
-      <c r="C21" s="52" t="s">
+      <c r="C21" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="D21" s="52" t="s">
-        <v>19</v>
-      </c>
-      <c r="E21" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="F21" s="52" t="s">
-        <v>7</v>
-      </c>
-      <c r="G21" s="31" t="s">
+      <c r="D21" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="G21" s="24" t="s">
         <v>205</v>
       </c>
-      <c r="H21" s="31" t="s">
+      <c r="H21" s="24" t="s">
         <v>206</v>
       </c>
       <c r="I21" s="7" t="s">
@@ -2864,27 +2855,27 @@
       <c r="A25" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="52">
+      <c r="B25" s="44">
         <v>36</v>
       </c>
-      <c r="C25" s="52" t="s">
+      <c r="C25" s="44" t="s">
         <v>268</v>
       </c>
-      <c r="D25" s="55" t="s">
+      <c r="D25" s="47" t="s">
+        <v>374</v>
+      </c>
+      <c r="E25" s="46"/>
+      <c r="F25" s="46"/>
+      <c r="G25" s="55" t="s">
+        <v>355</v>
+      </c>
+      <c r="H25" s="56" t="s">
         <v>375</v>
       </c>
-      <c r="E25" s="54"/>
-      <c r="F25" s="54"/>
-      <c r="G25" s="64" t="s">
-        <v>355</v>
-      </c>
-      <c r="H25" s="65" t="s">
-        <v>376</v>
-      </c>
-      <c r="I25" s="90" t="s">
-        <v>395</v>
-      </c>
-      <c r="J25" s="67" t="s">
+      <c r="I25" s="80" t="s">
+        <v>394</v>
+      </c>
+      <c r="J25" s="58" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2892,25 +2883,25 @@
       <c r="A26" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="66">
+      <c r="B26" s="57">
         <v>37</v>
       </c>
-      <c r="C26" s="66" t="s">
+      <c r="C26" s="57" t="s">
         <v>72</v>
       </c>
-      <c r="D26" s="66" t="s">
-        <v>19</v>
-      </c>
-      <c r="E26" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="F26" s="52" t="s">
-        <v>7</v>
-      </c>
-      <c r="G26" s="31" t="s">
+      <c r="D26" s="57" t="s">
+        <v>19</v>
+      </c>
+      <c r="E26" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26" s="24" t="s">
         <v>202</v>
       </c>
-      <c r="H26" s="31" t="s">
+      <c r="H26" s="24" t="s">
         <v>203</v>
       </c>
       <c r="I26" s="7" t="s">
@@ -3034,10 +3025,10 @@
         <v>7</v>
       </c>
       <c r="G30" s="9" t="s">
+        <v>389</v>
+      </c>
+      <c r="H30" s="9" t="s">
         <v>390</v>
-      </c>
-      <c r="H30" s="9" t="s">
-        <v>391</v>
       </c>
       <c r="I30" s="7" t="s">
         <v>165</v>
@@ -3210,26 +3201,26 @@
       <c r="A36" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B36" s="52">
+      <c r="B36" s="44">
         <v>51</v>
       </c>
-      <c r="C36" s="52" t="s">
+      <c r="C36" s="44" t="s">
         <v>95</v>
       </c>
-      <c r="D36" s="52" t="s">
-        <v>19</v>
-      </c>
-      <c r="E36" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="F36" s="52" t="s">
-        <v>7</v>
-      </c>
-      <c r="G36" s="60" t="s">
+      <c r="D36" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="E36" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="F36" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="G36" s="24" t="s">
         <v>204</v>
       </c>
-      <c r="H36" s="60" t="s">
-        <v>379</v>
+      <c r="H36" s="24" t="s">
+        <v>378</v>
       </c>
       <c r="I36" s="7" t="s">
         <v>27</v>
@@ -3353,10 +3344,10 @@
       <c r="F40" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G40" s="36" t="s">
+      <c r="G40" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="H40" s="36" t="s">
+      <c r="H40" s="29" t="s">
         <v>103</v>
       </c>
       <c r="I40" s="7" t="s">
@@ -3594,25 +3585,25 @@
       <c r="A48" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B48" s="52">
+      <c r="B48" s="44">
         <v>66</v>
       </c>
-      <c r="C48" s="52" t="s">
+      <c r="C48" s="44" t="s">
         <v>119</v>
       </c>
-      <c r="D48" s="52" t="s">
-        <v>19</v>
-      </c>
-      <c r="E48" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="F48" s="52" t="s">
-        <v>7</v>
-      </c>
-      <c r="G48" s="37" t="s">
+      <c r="D48" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="E48" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="F48" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="G48" s="30" t="s">
         <v>207</v>
       </c>
-      <c r="H48" s="37" t="s">
+      <c r="H48" s="30" t="s">
         <v>208</v>
       </c>
       <c r="I48" s="7" t="s">
@@ -3687,19 +3678,19 @@
       </c>
     </row>
     <row r="51" spans="1:10" ht="51" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="B51" s="21">
+      <c r="A51" s="82" t="s">
+        <v>5</v>
+      </c>
+      <c r="B51" s="84">
         <v>70</v>
       </c>
-      <c r="C51" s="21" t="s">
+      <c r="C51" s="84" t="s">
         <v>121</v>
       </c>
-      <c r="D51" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E51" s="23" t="s">
+      <c r="D51" s="82" t="s">
+        <v>19</v>
+      </c>
+      <c r="E51" s="86" t="s">
         <v>20</v>
       </c>
       <c r="F51" s="7" t="s">
@@ -3719,11 +3710,11 @@
       </c>
     </row>
     <row r="52" spans="1:10" ht="51" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="20"/>
-      <c r="B52" s="22"/>
-      <c r="C52" s="22"/>
-      <c r="D52" s="20"/>
-      <c r="E52" s="24"/>
+      <c r="A52" s="83"/>
+      <c r="B52" s="85"/>
+      <c r="C52" s="85"/>
+      <c r="D52" s="83"/>
+      <c r="E52" s="87"/>
       <c r="F52" s="7" t="s">
         <v>7</v>
       </c>
@@ -3827,7 +3818,7 @@
         <v>98</v>
       </c>
       <c r="H55" s="7" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="I55" s="7" t="s">
         <v>22</v>
@@ -3904,25 +3895,25 @@
       <c r="A58" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B58" s="68">
+      <c r="B58" s="59">
         <v>76</v>
       </c>
-      <c r="C58" s="69" t="s">
+      <c r="C58" s="60" t="s">
         <v>318</v>
       </c>
-      <c r="D58" s="70"/>
-      <c r="E58" s="70"/>
-      <c r="F58" s="70"/>
-      <c r="G58" s="71" t="s">
+      <c r="D58" s="61"/>
+      <c r="E58" s="61"/>
+      <c r="F58" s="61"/>
+      <c r="G58" s="62" t="s">
+        <v>376</v>
+      </c>
+      <c r="H58" s="51" t="s">
         <v>377</v>
-      </c>
-      <c r="H58" s="59" t="s">
-        <v>378</v>
       </c>
       <c r="I58" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="J58" s="67" t="s">
+      <c r="J58" s="58" t="s">
         <v>23</v>
       </c>
     </row>
@@ -4061,22 +4052,22 @@
       <c r="B63" s="8">
         <v>84</v>
       </c>
-      <c r="C63" s="52" t="s">
+      <c r="C63" s="44" t="s">
         <v>145</v>
       </c>
-      <c r="D63" s="52" t="s">
-        <v>19</v>
-      </c>
-      <c r="E63" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="F63" s="52" t="s">
-        <v>7</v>
-      </c>
-      <c r="G63" s="37" t="s">
+      <c r="D63" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="E63" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="F63" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="G63" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="H63" s="37" t="s">
+      <c r="H63" s="30" t="s">
         <v>209</v>
       </c>
       <c r="I63" s="7" t="s">
@@ -4093,22 +4084,22 @@
       <c r="B64" s="8">
         <v>85</v>
       </c>
-      <c r="C64" s="52" t="s">
+      <c r="C64" s="44" t="s">
         <v>146</v>
       </c>
-      <c r="D64" s="52" t="s">
-        <v>19</v>
-      </c>
-      <c r="E64" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="F64" s="52" t="s">
-        <v>7</v>
-      </c>
-      <c r="G64" s="37" t="s">
+      <c r="D64" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="E64" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="F64" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="G64" s="30" t="s">
         <v>210</v>
       </c>
-      <c r="H64" s="37" t="s">
+      <c r="H64" s="30" t="s">
         <v>211</v>
       </c>
       <c r="I64" s="7" t="s">
@@ -4125,22 +4116,22 @@
       <c r="B65" s="8">
         <v>86</v>
       </c>
-      <c r="C65" s="52" t="s">
+      <c r="C65" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="D65" s="52" t="s">
-        <v>19</v>
-      </c>
-      <c r="E65" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="F65" s="52" t="s">
-        <v>7</v>
-      </c>
-      <c r="G65" s="37" t="s">
+      <c r="D65" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="E65" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="F65" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="G65" s="30" t="s">
         <v>214</v>
       </c>
-      <c r="H65" s="37" t="s">
+      <c r="H65" s="30" t="s">
         <v>215</v>
       </c>
       <c r="I65" s="7" t="s">
@@ -4157,22 +4148,22 @@
       <c r="B66" s="8">
         <v>87</v>
       </c>
-      <c r="C66" s="52" t="s">
+      <c r="C66" s="44" t="s">
         <v>148</v>
       </c>
-      <c r="D66" s="52" t="s">
-        <v>19</v>
-      </c>
-      <c r="E66" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="F66" s="52" t="s">
-        <v>7</v>
-      </c>
-      <c r="G66" s="37" t="s">
+      <c r="D66" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="E66" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="F66" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="G66" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="H66" s="37" t="s">
+      <c r="H66" s="30" t="s">
         <v>213</v>
       </c>
       <c r="I66" s="7" t="s">
@@ -4189,22 +4180,22 @@
       <c r="B67" s="8">
         <v>88</v>
       </c>
-      <c r="C67" s="52" t="s">
+      <c r="C67" s="44" t="s">
         <v>149</v>
       </c>
-      <c r="D67" s="52" t="s">
-        <v>19</v>
-      </c>
-      <c r="E67" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="F67" s="52" t="s">
-        <v>7</v>
-      </c>
-      <c r="G67" s="37" t="s">
+      <c r="D67" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="E67" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="F67" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="G67" s="30" t="s">
         <v>210</v>
       </c>
-      <c r="H67" s="37" t="s">
+      <c r="H67" s="30" t="s">
         <v>211</v>
       </c>
       <c r="I67" s="7" t="s">
@@ -4221,22 +4212,22 @@
       <c r="B68" s="8">
         <v>89</v>
       </c>
-      <c r="C68" s="52" t="s">
+      <c r="C68" s="44" t="s">
         <v>150</v>
       </c>
-      <c r="D68" s="52" t="s">
-        <v>19</v>
-      </c>
-      <c r="E68" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="F68" s="52" t="s">
-        <v>7</v>
-      </c>
-      <c r="G68" s="37" t="s">
+      <c r="D68" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="E68" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="F68" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="G68" s="30" t="s">
         <v>210</v>
       </c>
-      <c r="H68" s="37" t="s">
+      <c r="H68" s="30" t="s">
         <v>211</v>
       </c>
       <c r="I68" s="7" t="s">
@@ -4253,23 +4244,23 @@
       <c r="B69" s="8">
         <v>92</v>
       </c>
-      <c r="C69" s="52" t="s">
+      <c r="C69" s="44" t="s">
         <v>151</v>
       </c>
-      <c r="D69" s="52" t="s">
-        <v>19</v>
-      </c>
-      <c r="E69" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="F69" s="52" t="s">
-        <v>7</v>
-      </c>
-      <c r="G69" s="31" t="s">
-        <v>371</v>
-      </c>
-      <c r="H69" s="52" t="s">
-        <v>393</v>
+      <c r="D69" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="E69" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="F69" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="G69" s="24" t="s">
+        <v>370</v>
+      </c>
+      <c r="H69" s="44" t="s">
+        <v>392</v>
       </c>
       <c r="I69" s="7" t="s">
         <v>22</v>
@@ -4317,22 +4308,22 @@
       <c r="B71" s="8">
         <v>95</v>
       </c>
-      <c r="C71" s="52" t="s">
+      <c r="C71" s="44" t="s">
         <v>153</v>
       </c>
-      <c r="D71" s="52" t="s">
-        <v>19</v>
-      </c>
-      <c r="E71" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="F71" s="52" t="s">
-        <v>7</v>
-      </c>
-      <c r="G71" s="37" t="s">
+      <c r="D71" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="E71" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="F71" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="G71" s="30" t="s">
         <v>210</v>
       </c>
-      <c r="H71" s="37" t="s">
+      <c r="H71" s="30" t="s">
         <v>211</v>
       </c>
       <c r="I71" s="7" t="s">
@@ -4349,22 +4340,22 @@
       <c r="B72" s="8">
         <v>96</v>
       </c>
-      <c r="C72" s="52" t="s">
+      <c r="C72" s="44" t="s">
         <v>154</v>
       </c>
-      <c r="D72" s="52" t="s">
-        <v>19</v>
-      </c>
-      <c r="E72" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="F72" s="52" t="s">
-        <v>7</v>
-      </c>
-      <c r="G72" s="37" t="s">
+      <c r="D72" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="E72" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="F72" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="G72" s="30" t="s">
         <v>214</v>
       </c>
-      <c r="H72" s="37" t="s">
+      <c r="H72" s="30" t="s">
         <v>215</v>
       </c>
       <c r="I72" s="7" t="s">
@@ -4381,22 +4372,22 @@
       <c r="B73" s="8">
         <v>97</v>
       </c>
-      <c r="C73" s="52" t="s">
+      <c r="C73" s="44" t="s">
         <v>155</v>
       </c>
-      <c r="D73" s="52" t="s">
-        <v>19</v>
-      </c>
-      <c r="E73" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="F73" s="52" t="s">
-        <v>7</v>
-      </c>
-      <c r="G73" s="37" t="s">
+      <c r="D73" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="E73" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="F73" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="G73" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="H73" s="37" t="s">
+      <c r="H73" s="30" t="s">
         <v>213</v>
       </c>
       <c r="I73" s="7" t="s">
@@ -4413,22 +4404,22 @@
       <c r="B74" s="8">
         <v>98</v>
       </c>
-      <c r="C74" s="52" t="s">
+      <c r="C74" s="44" t="s">
         <v>156</v>
       </c>
-      <c r="D74" s="52" t="s">
-        <v>19</v>
-      </c>
-      <c r="E74" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="F74" s="52" t="s">
-        <v>7</v>
-      </c>
-      <c r="G74" s="37" t="s">
+      <c r="D74" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="E74" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="F74" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="G74" s="30" t="s">
         <v>214</v>
       </c>
-      <c r="H74" s="37" t="s">
+      <c r="H74" s="30" t="s">
         <v>215</v>
       </c>
       <c r="I74" s="7" t="s">
@@ -4445,22 +4436,22 @@
       <c r="B75" s="8">
         <v>99</v>
       </c>
-      <c r="C75" s="52" t="s">
+      <c r="C75" s="44" t="s">
         <v>157</v>
       </c>
-      <c r="D75" s="52" t="s">
-        <v>19</v>
-      </c>
-      <c r="E75" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="F75" s="52" t="s">
-        <v>7</v>
-      </c>
-      <c r="G75" s="37" t="s">
+      <c r="D75" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="E75" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="F75" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="G75" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="H75" s="37" t="s">
+      <c r="H75" s="30" t="s">
         <v>213</v>
       </c>
       <c r="I75" s="7" t="s">
@@ -4477,22 +4468,22 @@
       <c r="B76" s="8">
         <v>102</v>
       </c>
-      <c r="C76" s="52" t="s">
+      <c r="C76" s="44" t="s">
         <v>158</v>
       </c>
-      <c r="D76" s="52" t="s">
-        <v>19</v>
-      </c>
-      <c r="E76" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="F76" s="52" t="s">
-        <v>7</v>
-      </c>
-      <c r="G76" s="37" t="s">
+      <c r="D76" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="E76" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="F76" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="G76" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="H76" s="37" t="s">
+      <c r="H76" s="30" t="s">
         <v>213</v>
       </c>
       <c r="I76" s="7" t="s">
@@ -4509,22 +4500,22 @@
       <c r="B77" s="8">
         <v>103</v>
       </c>
-      <c r="C77" s="52" t="s">
+      <c r="C77" s="44" t="s">
         <v>159</v>
       </c>
-      <c r="D77" s="52" t="s">
-        <v>19</v>
-      </c>
-      <c r="E77" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="F77" s="52" t="s">
-        <v>7</v>
-      </c>
-      <c r="G77" s="37" t="s">
+      <c r="D77" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="E77" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="F77" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="G77" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="H77" s="37" t="s">
+      <c r="H77" s="30" t="s">
         <v>213</v>
       </c>
       <c r="I77" s="7" t="s">
@@ -4575,8 +4566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F72AFE3-1E87-CF46-B503-516FB4ECE6EB}">
   <dimension ref="A2:D12"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="158" zoomScaleNormal="158" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="158" zoomScaleNormal="158" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4585,17 +4576,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.2">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="52" t="s">
         <v>363</v>
       </c>
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="63" t="s">
         <v>362</v>
       </c>
-      <c r="C2" s="61" t="s">
+      <c r="C2" s="52" t="s">
         <v>175</v>
       </c>
-      <c r="D2" s="61" t="s">
-        <v>380</v>
+      <c r="D2" s="52" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="112" x14ac:dyDescent="0.2">
@@ -4609,7 +4600,7 @@
         <v>354</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -4646,7 +4637,7 @@
         <v>234</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D6" s="17"/>
     </row>
@@ -4674,7 +4665,7 @@
       </c>
       <c r="D8" s="8"/>
     </row>
-    <row r="9" spans="1:4" s="12" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" s="12" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
         <v>12</v>
       </c>
@@ -4682,7 +4673,7 @@
         <v>171</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>369</v>
+        <v>400</v>
       </c>
       <c r="D9" s="8"/>
     </row>
@@ -4694,7 +4685,7 @@
         <v>172</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D10" s="7"/>
     </row>
@@ -4706,7 +4697,7 @@
         <v>173</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D11" s="7"/>
     </row>
@@ -4718,14 +4709,15 @@
         <v>174</v>
       </c>
       <c r="C12" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>373</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>374</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -4733,15 +4725,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB4D28A4-C67E-C24D-A558-9A5B7983454D}">
   <dimension ref="A2:G18"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="171" zoomScaleNormal="171" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="171" zoomScaleNormal="171" workbookViewId="0">
       <selection activeCell="A11" sqref="A3:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="20.1640625" style="39" customWidth="1"/>
-    <col min="3" max="3" width="19.83203125" style="39" customWidth="1"/>
-    <col min="4" max="4" width="21.1640625" style="48" customWidth="1"/>
+    <col min="2" max="2" width="20.1640625" style="31" customWidth="1"/>
+    <col min="3" max="3" width="19.83203125" style="31" customWidth="1"/>
+    <col min="4" max="4" width="21.1640625" style="40" customWidth="1"/>
     <col min="5" max="5" width="20.6640625" customWidth="1"/>
     <col min="6" max="6" width="24.6640625" customWidth="1"/>
     <col min="7" max="7" width="14.83203125" customWidth="1"/>
@@ -4749,62 +4741,62 @@
   <sheetData>
     <row r="2" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.2">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="33" t="s">
         <v>363</v>
       </c>
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="33" t="s">
         <v>362</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="33" t="s">
         <v>175</v>
       </c>
-      <c r="D3" s="49" t="s">
+      <c r="D3" s="41" t="s">
         <v>176</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="34" t="s">
         <v>176</v>
       </c>
-      <c r="F3" s="42" t="s">
+      <c r="F3" s="34" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.2">
-      <c r="A4" s="81">
+      <c r="A4" s="72">
         <v>2</v>
       </c>
-      <c r="B4" s="83" t="s">
+      <c r="B4" s="74" t="s">
         <v>228</v>
       </c>
-      <c r="C4" s="61" t="s">
+      <c r="C4" s="52" t="s">
+        <v>382</v>
+      </c>
+      <c r="D4" s="73" t="s">
+        <v>384</v>
+      </c>
+      <c r="E4" s="52" t="s">
         <v>383</v>
       </c>
-      <c r="D4" s="82" t="s">
-        <v>385</v>
-      </c>
-      <c r="E4" s="61" t="s">
-        <v>384</v>
-      </c>
-      <c r="F4" s="81">
+      <c r="F4" s="72">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="105" x14ac:dyDescent="0.2">
-      <c r="A5" s="43">
+      <c r="A5" s="35">
         <v>16</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="37" t="s">
         <v>243</v>
       </c>
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="37" t="s">
         <v>179</v>
       </c>
-      <c r="D5" s="50" t="s">
+      <c r="D5" s="42" t="s">
         <v>195</v>
       </c>
-      <c r="E5" s="45" t="s">
+      <c r="E5" s="37" t="s">
         <v>180</v>
       </c>
-      <c r="F5" s="44">
+      <c r="F5" s="36">
         <v>1</v>
       </c>
       <c r="G5" t="s">
@@ -4812,22 +4804,22 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="120" x14ac:dyDescent="0.2">
-      <c r="A6" s="47">
-        <v>19</v>
-      </c>
-      <c r="B6" s="47" t="s">
+      <c r="A6" s="39">
+        <v>19</v>
+      </c>
+      <c r="B6" s="39" t="s">
         <v>247</v>
       </c>
-      <c r="C6" s="45" t="s">
+      <c r="C6" s="37" t="s">
         <v>182</v>
       </c>
-      <c r="D6" s="50" t="s">
+      <c r="D6" s="42" t="s">
         <v>183</v>
       </c>
-      <c r="E6" s="45" t="s">
+      <c r="E6" s="37" t="s">
         <v>184</v>
       </c>
-      <c r="F6" s="46">
+      <c r="F6" s="38">
         <v>3</v>
       </c>
       <c r="G6" t="s">
@@ -4835,22 +4827,22 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.2">
-      <c r="A7" s="43">
-        <v>20</v>
-      </c>
-      <c r="B7" s="47" t="s">
+      <c r="A7" s="35">
+        <v>20</v>
+      </c>
+      <c r="B7" s="39" t="s">
         <v>249</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="C7" s="37" t="s">
         <v>185</v>
       </c>
-      <c r="D7" s="50" t="s">
+      <c r="D7" s="42" t="s">
         <v>220</v>
       </c>
-      <c r="E7" s="45" t="s">
+      <c r="E7" s="37" t="s">
         <v>186</v>
       </c>
-      <c r="F7" s="46">
+      <c r="F7" s="38">
         <v>4</v>
       </c>
       <c r="G7" t="s">
@@ -4858,91 +4850,91 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.2">
-      <c r="A8" s="43">
+      <c r="A8" s="35">
         <v>27</v>
       </c>
-      <c r="B8" s="47" t="s">
+      <c r="B8" s="39" t="s">
         <v>258</v>
       </c>
-      <c r="C8" s="45" t="s">
-        <v>389</v>
-      </c>
-      <c r="D8" s="50" t="s">
+      <c r="C8" s="37" t="s">
+        <v>388</v>
+      </c>
+      <c r="D8" s="42" t="s">
+        <v>386</v>
+      </c>
+      <c r="E8" s="37" t="s">
         <v>387</v>
       </c>
-      <c r="E8" s="45" t="s">
-        <v>388</v>
-      </c>
-      <c r="F8" s="46"/>
+      <c r="F8" s="38"/>
     </row>
     <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.2">
-      <c r="A9" s="43">
+      <c r="A9" s="35">
         <v>38</v>
       </c>
-      <c r="B9" s="47" t="s">
+      <c r="B9" s="39" t="s">
         <v>271</v>
       </c>
-      <c r="C9" s="45" t="s">
+      <c r="C9" s="37" t="s">
         <v>188</v>
       </c>
-      <c r="D9" s="50" t="s">
+      <c r="D9" s="42" t="s">
         <v>356</v>
       </c>
-      <c r="E9" s="45" t="s">
+      <c r="E9" s="37" t="s">
         <v>189</v>
       </c>
-      <c r="F9" s="46">
+      <c r="F9" s="38">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.2">
-      <c r="A10" s="43">
+      <c r="A10" s="35">
         <v>69</v>
       </c>
-      <c r="B10" s="47" t="s">
+      <c r="B10" s="39" t="s">
         <v>310</v>
       </c>
-      <c r="C10" s="45" t="s">
+      <c r="C10" s="37" t="s">
         <v>190</v>
       </c>
-      <c r="D10" s="50">
+      <c r="D10" s="42">
         <v>774893001</v>
       </c>
-      <c r="E10" s="45" t="s">
+      <c r="E10" s="37" t="s">
         <v>189</v>
       </c>
-      <c r="F10" s="46">
+      <c r="F10" s="38">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="90" x14ac:dyDescent="0.2">
-      <c r="A11" s="43">
+      <c r="A11" s="35">
         <v>101</v>
       </c>
-      <c r="B11" s="47" t="s">
+      <c r="B11" s="39" t="s">
         <v>350</v>
       </c>
-      <c r="C11" s="45" t="s">
+      <c r="C11" s="37" t="s">
         <v>191</v>
       </c>
-      <c r="D11" s="50" t="s">
+      <c r="D11" s="42" t="s">
         <v>192</v>
       </c>
-      <c r="E11" s="45" t="s">
+      <c r="E11" s="37" t="s">
         <v>193</v>
       </c>
-      <c r="F11" s="46">
+      <c r="F11" s="38">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
+      <c r="E17" s="88"/>
+      <c r="F17" s="88"/>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C18" s="40"/>
-      <c r="D18" s="51"/>
-      <c r="F18" s="39"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="43"/>
+      <c r="F18" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -6143,42 +6135,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="160" x14ac:dyDescent="0.2">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="19" t="s">
+        <v>395</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1" s="19" t="s">
         <v>396</v>
       </c>
-      <c r="B1" s="25" t="s">
-        <v>395</v>
-      </c>
-      <c r="C1" s="25" t="s">
+      <c r="D1" s="19" t="s">
         <v>397</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="E1" s="19" t="s">
         <v>398</v>
       </c>
-      <c r="E1" s="25" t="s">
-        <v>399</v>
-      </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="19" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="19" t="s">
         <v>357</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="19" t="s">
         <v>358</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="19" t="s">
         <v>359</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="19" t="s">
         <v>360</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="19" t="s">
         <v>361</v>
       </c>
-      <c r="F2" s="25"/>
+      <c r="F2" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6199,99 +6191,99 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3" ht="48" x14ac:dyDescent="0.2">
-      <c r="A2" s="80" t="s">
-        <v>382</v>
-      </c>
-      <c r="B2" s="73" t="s">
+      <c r="A2" s="71" t="s">
+        <v>381</v>
+      </c>
+      <c r="B2" s="64" t="s">
         <v>160</v>
       </c>
-      <c r="C2" s="74" t="s">
+      <c r="C2" s="65" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="75">
+      <c r="A3" s="66">
         <v>1</v>
       </c>
-      <c r="B3" s="76">
+      <c r="B3" s="67">
         <v>10</v>
       </c>
-      <c r="C3" s="77">
+      <c r="C3" s="68">
         <f>B3/B8</f>
         <v>0.10989010989010989</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="75">
+      <c r="A4" s="66">
         <v>2</v>
       </c>
-      <c r="B4" s="76">
+      <c r="B4" s="67">
         <v>30</v>
       </c>
-      <c r="C4" s="77">
+      <c r="C4" s="68">
         <f>B4/91</f>
         <v>0.32967032967032966</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="75">
+      <c r="A5" s="66">
         <v>3</v>
       </c>
-      <c r="B5" s="76">
+      <c r="B5" s="67">
         <v>0</v>
       </c>
-      <c r="C5" s="77">
+      <c r="C5" s="68">
         <f t="shared" ref="C5:C7" si="0">B5/91</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="75">
+      <c r="A6" s="66">
         <v>4</v>
       </c>
-      <c r="B6" s="76">
+      <c r="B6" s="67">
         <v>33</v>
       </c>
-      <c r="C6" s="77">
+      <c r="C6" s="68">
         <f t="shared" si="0"/>
         <v>0.36263736263736263</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="75">
-        <v>5</v>
-      </c>
-      <c r="B7" s="76">
+      <c r="A7" s="66">
+        <v>5</v>
+      </c>
+      <c r="B7" s="67">
         <v>18</v>
       </c>
-      <c r="C7" s="77">
+      <c r="C7" s="68">
         <f t="shared" si="0"/>
         <v>0.19780219780219779</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="78" t="s">
+      <c r="A8" s="69" t="s">
         <v>160</v>
       </c>
-      <c r="B8" s="79">
+      <c r="B8" s="70">
         <f>SUM(B3:B7)</f>
         <v>91</v>
       </c>
-      <c r="C8" s="77">
+      <c r="C8" s="68">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>394</v>
-      </c>
-      <c r="B10" s="85">
+        <v>393</v>
+      </c>
+      <c r="B10" s="75">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B11">
         <f>B8+12</f>

</xml_diff>